<commit_message>
Save data validations to worksheet extensions
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Misc/DataValidation.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Misc/DataValidation.xlsx
@@ -504,7 +504,7 @@
       <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A5:A5">
-      <x:formula1>'Data Validation'!$C$1:$C$2</x:formula1>
+      <x:formula1>$C$1:$C$2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A6:A6">
@@ -688,7 +688,7 @@
       </x:c>
     </x:row>
   </x:sheetData>
-  <x:dataValidations count="7">
+  <x:dataValidations count="6">
     <x:dataValidation type="decimal" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A1">
       <x:formula1>1</x:formula1>
       <x:formula2>5</x:formula2>
@@ -699,10 +699,6 @@
     </x:dataValidation>
     <x:dataValidation type="date" errorStyle="stop" operator="greaterThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="Can't party like it's 1999." prompt="Please enter a date in this century." sqref="A4:A4">
       <x:formula1>36526</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A5:A5">
-      <x:formula1>'Data Validation'!$C$1:$C$2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A6:A6">
@@ -730,6 +726,18 @@
     <x:firstFooter/>
   </x:headerFooter>
   <x:tableParts count="0"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="">
+          <x14:formula1>
+            <xm:f>'Data Validation'!$C$1:$C$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>A5:A5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </x:ext>
+  </x:extLst>
 </x:worksheet>
 </file>
 
@@ -900,7 +908,7 @@
       </x:c>
     </x:row>
   </x:sheetData>
-  <x:dataValidations count="7">
+  <x:dataValidations count="6">
     <x:dataValidation type="decimal" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A1">
       <x:formula1>1</x:formula1>
       <x:formula2>5</x:formula2>
@@ -911,10 +919,6 @@
     </x:dataValidation>
     <x:dataValidation type="date" errorStyle="stop" operator="greaterThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="Can't party like it's 1999." prompt="Please enter a date in this century." sqref="A4:A4">
       <x:formula1>36526</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A5:A5">
-      <x:formula1>'Data Validation'!$C$1:$C$2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A6:A6">
@@ -935,6 +939,18 @@
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="0"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="">
+          <x14:formula1>
+            <xm:f>'Data Validation'!$C$1:$C$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>A5:A5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </x:ext>
+  </x:extLst>
 </x:worksheet>
 </file>
 

</xml_diff>

<commit_message>
Don't calculate count of data validations twice. Set the `count` attribute in data validation extensions to the correct value instead of a stale value.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Misc/DataValidation.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Misc/DataValidation.xlsx
@@ -728,7 +728,7 @@
   <x:tableParts count="0"/>
   <x:extLst>
     <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="">
           <x14:formula1>
             <xm:f>'Data Validation'!$C$1:$C$2</xm:f>
@@ -941,7 +941,7 @@
   <x:tableParts count="0"/>
   <x:extLst>
     <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="">
           <x14:formula1>
             <xm:f>'Data Validation'!$C$1:$C$2</xm:f>

</xml_diff>

<commit_message>
Update reference file: only order of data validation rules on sheet6 changed
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Misc/DataValidation.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Misc/DataValidation.xlsx
@@ -1055,33 +1055,33 @@
       <x:formula1>1.1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="notEqual" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
+      <x:formula1>2.2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="greaterThan" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B12">
+      <x:formula1>3.3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="lessThan" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D6">
+      <x:formula1>4.4</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="greaterThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C14">
+      <x:formula1>5.5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="lessThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D12">
+      <x:formula1>6.6</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5">
+      <x:formula1>7.7</x:formula1>
+      <x:formula2>8.8</x:formula2>
+    </x:dataValidation>
     <x:dataValidation type="decimal" errorStyle="stop" operator="notBetween" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="H1:H12">
       <x:formula1>9.9</x:formula1>
       <x:formula2>10.1</x:formula2>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="greaterThan" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B12">
-      <x:formula1>3.3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5">
-      <x:formula1>7.7</x:formula1>
-      <x:formula2>8.8</x:formula2>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="lessThan" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D6">
-      <x:formula1>4.4</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="notEqual" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
-      <x:formula1>2.2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="lessThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D12">
-      <x:formula1>6.6</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="greaterThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C14">
-      <x:formula1>5.5</x:formula1>
-      <x:formula2/>
     </x:dataValidation>
   </x:dataValidations>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>